<commit_message>
Deploying to gh-pages from @ jrybak23/directories-generator@331b45b2bd9d37e4545087fd85ef0173b553e0d0 🚀
</commit_message>
<xml_diff>
--- a/app/excel-reader/test-assets/test.spec.xlsx
+++ b/app/excel-reader/test-assets/test.spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ihor_Rybak\IdeaProjects\directories-generator\src\app\excel-reader\test-assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7CA145-AB88-40E2-AE8D-39E1A5C76702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F9C87-2E01-4110-8DC8-D462CD8A7DDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9D5E9BD5-0DA2-4C83-8E97-6CCCD01D87AB}"/>
+    <workbookView xWindow="1692" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{9D5E9BD5-0DA2-4C83-8E97-6CCCD01D87AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>v22</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>v43</t>
+  </si>
+  <si>
+    <t>v61</t>
+  </si>
+  <si>
+    <t>v71</t>
+  </si>
+  <si>
+    <t>v91</t>
+  </si>
+  <si>
+    <t>v11_1</t>
+  </si>
+  <si>
+    <t>v12_2</t>
   </si>
 </sst>
 </file>
@@ -421,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBDB503-63CD-45B8-B42B-C9C86F5A3CB6}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,6 +490,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>